<commit_message>
Add Current Sense BOM
</commit_message>
<xml_diff>
--- a/Master_Board/V1/BOM/Master_Digikey.xlsx
+++ b/Master_Board/V1/BOM/Master_Digikey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\Hardware\EclipseX-BMS-Hardware\Master_Board\V1\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\EclipseX-BMS-Hardware\Master_Board\V1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>B240AQ-13-FDICT-ND</t>
   </si>
@@ -354,6 +354,51 @@
   </si>
   <si>
     <t>535-10212-1-ND</t>
+  </si>
+  <si>
+    <t>MAX9938FEUK+T</t>
+  </si>
+  <si>
+    <t>Maxim Integrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX9938FEUK+TCT-ND </t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>BMS_Master</t>
+  </si>
+  <si>
+    <t>PowerSupplyX</t>
+  </si>
+  <si>
+    <t>RL1206FR-7W0R01L</t>
+  </si>
+  <si>
+    <t>311-.01LYCT-ND</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>732-1942-ND</t>
+  </si>
+  <si>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>BMS_Slave</t>
+  </si>
+  <si>
+    <t>732-1944-ND</t>
+  </si>
+  <si>
+    <t>64900713722DEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-4891-ND </t>
   </si>
 </sst>
 </file>
@@ -362,7 +407,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_)\ _$_ ;_ * \(#,##0.00\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_)\ _$_ ;_ * \(#,##0\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_)\ _$_ ;_ * \(#,##0\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -442,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,12 +498,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -741,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,10 +803,11 @@
     <col min="2" max="2" width="33" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
+    <col min="5" max="5" width="21" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -770,20 +821,23 @@
         <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,22 +850,25 @@
       <c r="D2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.59</v>
       </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G43" si="0">E2*F2</f>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H48" si="0">F2*G2</f>
         <v>0.59</v>
       </c>
-      <c r="I2" s="1">
-        <f>SUM(G2:G43)</f>
-        <v>140.53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <f>SUM(H2:H48)</f>
+        <v>156.47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -824,18 +881,21 @@
       <c r="D3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -848,18 +908,21 @@
       <c r="D4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>1.32</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
         <v>5.28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -872,18 +935,21 @@
       <c r="D5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.24</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -896,18 +962,21 @@
       <c r="D6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.59</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>1.77</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -920,18 +989,21 @@
       <c r="D7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>1.32</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>2.64</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -944,18 +1016,21 @@
       <c r="D8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>3.16</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>3.16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -968,18 +1043,21 @@
       <c r="D9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>4.55</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -992,18 +1070,21 @@
       <c r="D10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.21</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1016,18 +1097,21 @@
       <c r="D11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="1">
         <v>6</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>0.16</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1040,18 +1124,21 @@
       <c r="D12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>0.65</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>1.9500000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1064,18 +1151,21 @@
       <c r="D13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>0.15</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1088,18 +1178,21 @@
       <c r="D14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="1">
         <v>10</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.15</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1112,18 +1205,21 @@
       <c r="D15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="1">
         <v>10</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>0.15</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1136,18 +1232,21 @@
       <c r="D16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="1">
         <v>20</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>0.15</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1160,18 +1259,21 @@
       <c r="D17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.15</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1184,18 +1286,21 @@
       <c r="D18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="1">
         <v>10</v>
       </c>
-      <c r="F18" s="5">
+      <c r="G18" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1208,18 +1313,21 @@
       <c r="D19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="1">
         <v>10</v>
       </c>
-      <c r="F19" s="5">
+      <c r="G19" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1232,18 +1340,21 @@
       <c r="D20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="1">
         <v>10</v>
       </c>
-      <c r="F20" s="5">
+      <c r="G20" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1256,18 +1367,21 @@
       <c r="D21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="1">
         <v>10</v>
       </c>
-      <c r="F21" s="5">
+      <c r="G21" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1280,18 +1394,21 @@
       <c r="D22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>0.15</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1304,18 +1421,21 @@
       <c r="D23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="1">
         <v>10</v>
       </c>
-      <c r="F23" s="5">
+      <c r="G23" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1328,18 +1448,21 @@
       <c r="D24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>0.15</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1352,18 +1475,21 @@
       <c r="D25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="1">
         <v>10</v>
       </c>
-      <c r="F25" s="5">
+      <c r="G25" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1376,18 +1502,21 @@
       <c r="D26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="1">
         <v>10</v>
       </c>
-      <c r="F26" s="5">
+      <c r="G26" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1400,18 +1529,21 @@
       <c r="D27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="1">
         <v>10</v>
       </c>
-      <c r="F27" s="5">
+      <c r="G27" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1424,18 +1556,21 @@
       <c r="D28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="1">
         <v>10</v>
       </c>
-      <c r="F28" s="5">
+      <c r="G28" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1448,18 +1583,21 @@
       <c r="D29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>0.63</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1472,18 +1610,21 @@
       <c r="D30" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>5.64</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <f t="shared" si="0"/>
         <v>11.28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1496,18 +1637,21 @@
       <c r="D31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="1">
         <v>2</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>3.24</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <f t="shared" si="0"/>
         <v>6.48</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1520,18 +1664,21 @@
       <c r="D32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="1">
         <v>4</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>8.74</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <f t="shared" si="0"/>
         <v>34.96</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1544,18 +1691,21 @@
       <c r="D33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>0.18</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1568,18 +1718,21 @@
       <c r="D34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="1">
         <v>2</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>0.23</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1592,18 +1745,21 @@
       <c r="D35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="1">
         <v>2</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>10.029999999999999</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <f t="shared" si="0"/>
         <v>20.059999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1616,18 +1772,21 @@
       <c r="D36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1">
         <v>1</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>1.38</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <f t="shared" si="0"/>
         <v>1.38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1640,18 +1799,21 @@
       <c r="D37" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="1">
         <v>1</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1664,18 +1826,21 @@
       <c r="D38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="1">
         <v>4</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>0.63</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <f t="shared" si="0"/>
         <v>2.52</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -1688,18 +1853,21 @@
       <c r="D39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="1">
         <v>1</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>11.92</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <f t="shared" si="0"/>
         <v>11.92</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1712,18 +1880,21 @@
       <c r="D40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="1">
         <v>1</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>6.06</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <f t="shared" si="0"/>
         <v>6.06</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -1736,18 +1907,21 @@
       <c r="D41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="1">
         <v>2</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="1">
         <v>2.69</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <f t="shared" si="0"/>
         <v>5.38</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>109</v>
       </c>
@@ -1760,18 +1934,21 @@
       <c r="D42" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="1">
         <v>1</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="1">
         <v>0.38</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -1784,15 +1961,153 @@
       <c r="D43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="1">
         <v>1</v>
       </c>
-      <c r="F43" s="2">
+      <c r="G43" s="1">
         <v>0.6</v>
       </c>
-      <c r="G43" s="2">
+      <c r="H43" s="1">
         <f t="shared" si="0"/>
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2.27</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="0"/>
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="4">
+        <v>649002113322</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="1">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3400000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="4">
+        <v>649006113322</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="0"/>
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="1">
+        <v>50</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.1096</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="0"/>
+        <v>5.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>